<commit_message>
StudentMAster and TeacherAttendancemaster change done
</commit_message>
<xml_diff>
--- a/InvoiceManagementSystem/Data/BulkStudent/DemoBulkStudent.xlsx
+++ b/InvoiceManagementSystem/Data/BulkStudent/DemoBulkStudent.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Title</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>panchalveer@gmail.com</t>
-  </si>
-  <si>
-    <t>1st</t>
   </si>
   <si>
     <t>MBA</t>
@@ -509,7 +506,7 @@
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -534,7 +531,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -570,34 +567,34 @@
         <v>11</v>
       </c>
       <c r="N1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
         <v>34</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>35</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>37</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>38</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>39</v>
-      </c>
-      <c r="T1" t="s">
-        <v>40</v>
       </c>
       <c r="U1" t="s">
         <v>12</v>
       </c>
       <c r="V1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="W1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X1" t="s">
         <v>13</v>
@@ -626,19 +623,19 @@
     </row>
     <row r="2" spans="1:31">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
       </c>
       <c r="F2" t="s">
         <v>21</v>
@@ -658,26 +655,26 @@
       <c r="L2" s="1">
         <v>45322</v>
       </c>
-      <c r="M2" t="s">
-        <v>23</v>
+      <c r="M2">
+        <v>1</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" t="s">
         <v>42</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>43</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>44</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="T2">
         <v>8487521365</v>
@@ -686,34 +683,34 @@
         <v>39844</v>
       </c>
       <c r="V2" t="s">
+        <v>23</v>
+      </c>
+      <c r="W2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" t="s">
         <v>24</v>
-      </c>
-      <c r="W2" t="s">
-        <v>47</v>
-      </c>
-      <c r="X2" t="s">
-        <v>25</v>
       </c>
       <c r="Y2">
         <v>382443</v>
       </c>
       <c r="Z2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" t="s">
         <v>26</v>
       </c>
-      <c r="AA2" t="s">
-        <v>27</v>
-      </c>
       <c r="AB2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AC2">
         <v>382443</v>
       </c>
       <c r="AD2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE2" t="s">
         <v>26</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>